<commit_message>
beofre pull 27 april 2023
</commit_message>
<xml_diff>
--- a/LOGS/ee28273f-763a-4806-85e9-90d78e717975/main_page_service_output/notes_cropped_df.xlsx
+++ b/LOGS/ee28273f-763a-4806-85e9-90d78e717975/main_page_service_output/notes_cropped_df.xlsx
@@ -31,18 +31,17 @@
     <sheet name="26__fbd390e7-20b7-3f" sheetId="22" r:id="rId22"/>
     <sheet name="26__fd32b450-dd14-34" sheetId="23" r:id="rId23"/>
     <sheet name="27__ad70d8e4-65c2-37" sheetId="24" r:id="rId24"/>
-    <sheet name="5__264918a9-ada8-3ad" sheetId="25" r:id="rId25"/>
-    <sheet name="7__2b6c970d-d737-3d6" sheetId="26" r:id="rId26"/>
-    <sheet name="8__2b6c970d-d737-3d6" sheetId="27" r:id="rId27"/>
-    <sheet name="9__2b6c970d-d737-3d6" sheetId="28" r:id="rId28"/>
-    <sheet name="9__d8765e27-2250-395" sheetId="29" r:id="rId29"/>
+    <sheet name="7__2b6c970d-d737-3d6" sheetId="25" r:id="rId25"/>
+    <sheet name="8__2b6c970d-d737-3d6" sheetId="26" r:id="rId26"/>
+    <sheet name="9__2b6c970d-d737-3d6" sheetId="27" r:id="rId27"/>
+    <sheet name="9__d8765e27-2250-395" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="347">
   <si>
     <t>2022 $</t>
   </si>
@@ -978,33 +977,6 @@
   </si>
   <si>
     <t>2903041</t>
-  </si>
-  <si>
-    <t>Crane sales</t>
-  </si>
-  <si>
-    <t>After service and parts sales</t>
-  </si>
-  <si>
-    <t>Total Revenue</t>
-  </si>
-  <si>
-    <t>128008786</t>
-  </si>
-  <si>
-    <t>16051994</t>
-  </si>
-  <si>
-    <t>144417994</t>
-  </si>
-  <si>
-    <t>146106970</t>
-  </si>
-  <si>
-    <t>13700633</t>
-  </si>
-  <si>
-    <t>160803224</t>
   </si>
   <si>
     <t>7. Other gains and losses</t>
@@ -2978,13 +2950,13 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -2994,54 +2966,65 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>312</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>313</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>312</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
         <v>315</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B5" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>314</v>
-      </c>
-      <c r="B6" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" t="s">
-        <v>320</v>
+      <c r="D6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3072,60 +3055,54 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B2" t="s">
-        <v>321</v>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" t="s">
-        <v>322</v>
-      </c>
       <c r="C3" t="s">
-        <v>325</v>
-      </c>
-      <c r="D3" t="s">
-        <v>329</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="C6" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
+      <c r="A7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B7" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3156,16 +3133,19 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="C3" t="s">
         <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3176,7 +3156,7 @@
         <v>337</v>
       </c>
       <c r="D4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3187,23 +3167,26 @@
         <v>338</v>
       </c>
       <c r="D5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>336</v>
+      </c>
       <c r="C6" t="s">
         <v>339</v>
       </c>
       <c r="D6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B7" t="s">
-        <v>336</v>
+      <c r="C7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3212,90 +3195,6 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>333</v>
-      </c>
-      <c r="B2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>343</v>
-      </c>
-      <c r="C4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C5" t="s">
-        <v>347</v>
-      </c>
-      <c r="D5" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" t="s">
-        <v>345</v>
-      </c>
-      <c r="C6" t="s">
-        <v>348</v>
-      </c>
-      <c r="D6" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
-        <v>349</v>
-      </c>
-      <c r="D7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3324,7 +3223,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B3">
         <v>383044</v>
@@ -3335,7 +3234,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B4">
         <v>166547</v>

</xml_diff>